<commit_message>
Connexion et Gestion du mot de passe
Mise en place de la connexion et de la gestion du mot de passe oublié.
Début de l'implémentation du formulaire de modification du compte avec la photo de profil
</commit_message>
<xml_diff>
--- a/docs/Tableau_MVC.xlsx
+++ b/docs/Tableau_MVC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\front\exercices\exercices-back\exercice-pizza\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5325E446-816D-437D-B714-2BF4970849E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17F407C-8C57-4539-88C5-B56ACFA8EB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modèles" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
   <si>
     <t>Rôle</t>
   </si>
@@ -294,6 +294,26 @@
   </si>
   <si>
     <t>Footer de la page HTML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modifier le profil de l'utilisateur </t>
+  </si>
+  <si>
+    <t>modifier_utilisateur.php</t>
+  </si>
+  <si>
+    <t>GET - id - Identifiant de l'utilisateur à modifier
+POST - action - Informations sur le profil</t>
+  </si>
+  <si>
+    <t>Afficher le formulaire de gestion du profil</t>
+  </si>
+  <si>
+    <t>afficher_form_utilisateur.php</t>
+  </si>
+  <si>
+    <t>GET - id - Facultatif - Identifiant d'un utilisateur
+GET - action - Action à réaliser</t>
   </si>
 </sst>
 </file>
@@ -799,7 +819,7 @@
   </sheetPr>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -1026,10 +1046,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,119 +1188,135 @@
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>6</v>
+        <v>88</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>56</v>
+      <c r="C11" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>57</v>
+        <v>17</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>58</v>
+        <v>17</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>69</v>
+        <v>57</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>71</v>
+      <c r="C15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
+      <c r="D19" s="6"/>
     </row>
     <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
@@ -1295,13 +1331,13 @@
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
+      <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
+      <c r="D22" s="6"/>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
+      <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="7"/>
@@ -1315,38 +1351,38 @@
     <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="5"/>
+      <c r="C25" s="6"/>
       <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
+      <c r="A26" s="10"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
     </row>
-    <row r="27" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
+    <row r="27" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
+      <c r="C27" s="5"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
+    <row r="28" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
+      <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
@@ -1376,49 +1412,49 @@
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
+      <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
+      <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
-      <c r="D37" s="4"/>
+      <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
-      <c r="D38" s="4"/>
+      <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
+      <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
+      <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
-      <c r="D41" s="4"/>
+      <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
-      <c r="D42" s="4"/>
+      <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
@@ -1456,6 +1492,18 @@
       <c r="C48" s="3"/>
       <c r="D48" s="4"/>
     </row>
+    <row r="49" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Début du formulaire de Pizza
</commit_message>
<xml_diff>
--- a/docs/Tableau_MVC.xlsx
+++ b/docs/Tableau_MVC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\front\exercices\exercices-back\exercice-pizza\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17F407C-8C57-4539-88C5-B56ACFA8EB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F373B2-F181-4DBB-868F-039661FFD8B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="96">
   <si>
     <t>Rôle</t>
   </si>
@@ -212,9 +212,6 @@
     <t>supprimer_pizza.php</t>
   </si>
   <si>
-    <t>lister_ingredients.php</t>
-  </si>
-  <si>
     <t>finaliser_commande.php</t>
   </si>
   <si>
@@ -250,9 +247,6 @@
     <t>REQUEST - tableau - Paramètres de filtre pour afficher les ingrédients</t>
   </si>
   <si>
-    <t>Retourne la liste des ingrédients</t>
-  </si>
-  <si>
     <t>Finalise la commande</t>
   </si>
   <si>
@@ -314,6 +308,21 @@
   <si>
     <t>GET - id - Facultatif - Identifiant d'un utilisateur
 GET - action - Action à réaliser</t>
+  </si>
+  <si>
+    <t>lister_compositions.php</t>
+  </si>
+  <si>
+    <t>Retourne la liste de la composition de la pizza</t>
+  </si>
+  <si>
+    <t>Récupérer le formulaire pour ajouter une composition</t>
+  </si>
+  <si>
+    <t>afficher_form_composition.php</t>
+  </si>
+  <si>
+    <t>GET - type - Facultatif - Type de l'ingrédient pour filtrer le formulaire</t>
   </si>
 </sst>
 </file>
@@ -349,7 +358,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -364,12 +373,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -407,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -436,11 +439,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -842,38 +848,38 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C5" s="4"/>
     </row>
@@ -888,11 +894,11 @@
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:3" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -951,21 +957,21 @@
     </row>
     <row r="14" spans="1:3" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>43</v>
@@ -1048,8 +1054,8 @@
   </sheetPr>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,35 +1194,35 @@
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>17</v>
@@ -1230,7 +1236,7 @@
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>17</v>
@@ -1239,12 +1245,12 @@
         <v>56</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>18</v>
@@ -1253,12 +1259,12 @@
         <v>57</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>18</v>
@@ -1267,12 +1273,12 @@
         <v>58</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>18</v>
@@ -1281,42 +1287,50 @@
         <v>59</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="A19" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
@@ -1337,73 +1351,73 @@
       <c r="D22" s="6"/>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
+      <c r="A27" s="11"/>
       <c r="B27" s="6"/>
       <c r="C27" s="5"/>
       <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="7"/>
     </row>
     <row r="29" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
+      <c r="A34" s="12"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="4"/>

</xml_diff>